<commit_message>
Major progress on code cleanup #36  and Standardization #37
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F7F3D-A118-47B0-AA81-FA248BE7FB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB8E242-2448-40EC-A887-FC39F9CCC2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoint Implementation Status" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="466">
   <si>
     <t>Namespace</t>
   </si>
@@ -1433,6 +1433,12 @@
   </si>
   <si>
     <t>TVSeasonEpisodes</t>
+  </si>
+  <si>
+    <t>ITMDBDiscoverMoviePage</t>
+  </si>
+  <si>
+    <t>ITMDBDiscoverTVPage</t>
   </si>
 </sst>
 </file>
@@ -1913,9 +1919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB394B0-4279-4C9C-A2E8-1B3086916310}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H108" sqref="H108"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,6 +2832,9 @@
       <c r="E39" t="s">
         <v>132</v>
       </c>
+      <c r="F39" t="s">
+        <v>464</v>
+      </c>
       <c r="G39" s="4" t="s">
         <v>78</v>
       </c>
@@ -2848,6 +2857,9 @@
       </c>
       <c r="E40" t="s">
         <v>133</v>
+      </c>
+      <c r="F40" t="s">
+        <v>465</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>78</v>
@@ -5498,9 +5510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449EFBB5-22F1-48B7-A5F5-01E59CD1CC21}">
   <dimension ref="A1:M203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7105,11 +7117,11 @@
       <c r="C36" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>78</v>
+      <c r="D36" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>459</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>78</v>
@@ -7152,11 +7164,11 @@
       <c r="C37" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>78</v>
+      <c r="D37" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>459</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Implemented rate limiting #40
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C978D9F3-F55B-4B42-A1CB-EAE69C50710C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE9B7A7-4DA4-46C8-B010-5548BE35FA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="449">
   <si>
     <t>Namespace</t>
   </si>
@@ -1869,8 +1869,8 @@
   <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,7 +2998,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3252,14 +3252,11 @@
       <c r="F60" t="s">
         <v>205</v>
       </c>
-      <c r="G60" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H60" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G60" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3282,7 +3279,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3305,7 +3302,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3328,7 +3325,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Progress on People #26
- Implemented People - GetChanges
- Implemented People - GetExternalIDs
- Implemented People - GetImages
- Implemented People - GetLatest
- Implemented People - GetTranslations
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A057C-0682-4005-806C-B9487672CA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CA9873-82FF-4B9F-8650-DAABC268FCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoint Implementation Status" sheetId="1" r:id="rId1"/>
@@ -1877,9 +1877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB394B0-4279-4C9C-A2E8-1B3086916310}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,8 +3813,8 @@
       <c r="F84" t="s">
         <v>78</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>74</v>
+      <c r="G84" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3856,8 +3856,8 @@
       <c r="F86" t="s">
         <v>212</v>
       </c>
-      <c r="G86" s="4" t="s">
-        <v>74</v>
+      <c r="G86" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3879,8 +3879,8 @@
       <c r="F87" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="4" t="s">
-        <v>74</v>
+      <c r="G87" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3902,8 +3902,8 @@
       <c r="F88" t="s">
         <v>226</v>
       </c>
-      <c r="G88" s="4" t="s">
-        <v>74</v>
+      <c r="G88" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3985,8 +3985,8 @@
       <c r="F92" t="s">
         <v>102</v>
       </c>
-      <c r="G92" s="4" t="s">
-        <v>74</v>
+      <c r="G92" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -5359,8 +5359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449EFBB5-22F1-48B7-A5F5-01E59CD1CC21}">
   <dimension ref="A1:M204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented Media Watch Providers #35
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B882D4B6-6D65-40BE-A9CF-AD0C7714B895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422EB1F5-A85E-42B4-AB14-8555122FFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2452" uniqueCount="491">
   <si>
     <t>Namespace</t>
   </si>
@@ -1404,9 +1404,6 @@
     <t>ITMDBEpisodeDetail</t>
   </si>
   <si>
-    <t>ITMDBMediaWatchProviders</t>
-  </si>
-  <si>
     <t>GetDetail</t>
   </si>
   <si>
@@ -1510,6 +1507,15 @@
   </si>
   <si>
     <t>CombinedCrewCredits</t>
+  </si>
+  <si>
+    <t>MediaWatchProviderCountry</t>
+  </si>
+  <si>
+    <t>MediaWatchProviderCountries</t>
+  </si>
+  <si>
+    <t>TTMDBMediaWatchProviderCountries</t>
   </si>
 </sst>
 </file>
@@ -1986,8 +1992,8 @@
   <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,7 +2003,7 @@
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.42578125" customWidth="1"/>
   </cols>
@@ -3735,10 +3741,10 @@
         <v>207</v>
       </c>
       <c r="F76" t="s">
-        <v>453</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>74</v>
+        <v>490</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3942,7 +3948,7 @@
         <v>222</v>
       </c>
       <c r="F85" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>255</v>
@@ -4034,7 +4040,7 @@
         <v>223</v>
       </c>
       <c r="F89" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>255</v>
@@ -4057,7 +4063,7 @@
         <v>224</v>
       </c>
       <c r="F90" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>255</v>
@@ -4928,10 +4934,10 @@
         <v>207</v>
       </c>
       <c r="F128" t="s">
-        <v>453</v>
-      </c>
-      <c r="G128" s="4" t="s">
-        <v>74</v>
+        <v>490</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4988,7 +4994,7 @@
         <v>3</v>
       </c>
       <c r="E131" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F131" t="s">
         <v>451</v>
@@ -5198,10 +5204,10 @@
         <v>207</v>
       </c>
       <c r="F140" t="s">
-        <v>453</v>
-      </c>
-      <c r="G140" s="4" t="s">
-        <v>74</v>
+        <v>490</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -5218,7 +5224,7 @@
         <v>3</v>
       </c>
       <c r="E141" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F141" t="s">
         <v>452</v>
@@ -5528,11 +5534,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449EFBB5-22F1-48B7-A5F5-01E59CD1CC21}">
-  <dimension ref="A1:M186"/>
+  <dimension ref="A1:M188"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D143" sqref="D143"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F184" sqref="F184:F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9684,7 +9690,7 @@
         <v>93</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>267</v>
@@ -9731,7 +9737,7 @@
         <v>93</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>268</v>
@@ -9778,7 +9784,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>267</v>
@@ -9825,7 +9831,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>268</v>
@@ -9872,7 +9878,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>323</v>
@@ -9919,7 +9925,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>324</v>
@@ -9966,7 +9972,7 @@
         <v>93</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>325</v>
@@ -10013,7 +10019,7 @@
         <v>93</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>326</v>
@@ -10060,7 +10066,7 @@
         <v>93</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D99" s="14" t="s">
         <v>377</v>
@@ -10104,7 +10110,7 @@
         <v>93</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>272</v>
@@ -10151,7 +10157,7 @@
         <v>93</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>273</v>
@@ -10198,7 +10204,7 @@
         <v>93</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>272</v>
@@ -10245,7 +10251,7 @@
         <v>93</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>273</v>
@@ -10292,7 +10298,7 @@
         <v>93</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>377</v>
@@ -11546,7 +11552,7 @@
         <v>176</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C131" s="10" t="s">
         <v>267</v>
@@ -11593,7 +11599,7 @@
         <v>176</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C132" s="10" t="s">
         <v>268</v>
@@ -12312,11 +12318,11 @@
         <v>TTMDBWatchProviderPriority</v>
       </c>
       <c r="I147" s="8" t="str">
-        <f t="shared" ref="I147:I186" si="86">"  "&amp;G147&amp;" = interface;"</f>
+        <f t="shared" ref="I147:I188" si="86">"  "&amp;G147&amp;" = interface;"</f>
         <v xml:space="preserve">  ITMDBWatchProviderPriority = interface;</v>
       </c>
       <c r="J147" s="8" t="str">
-        <f t="shared" ref="J147:J186" si="87">"  "&amp;H147&amp;" = class;"</f>
+        <f t="shared" ref="J147:J188" si="87">"  "&amp;H147&amp;" = class;"</f>
         <v xml:space="preserve">  TTMDBWatchProviderPriority = class;</v>
       </c>
       <c r="K147" s="8" t="str">
@@ -12395,11 +12401,11 @@
         <v>74</v>
       </c>
       <c r="G149" s="8" t="str">
-        <f t="shared" ref="G149:G181" si="88">"I"&amp;M149&amp;B149</f>
+        <f t="shared" ref="G149:G183" si="88">"I"&amp;M149&amp;B149</f>
         <v>ITMDBWatchProvider</v>
       </c>
       <c r="H149" s="8" t="str">
-        <f t="shared" ref="H149:H181" si="89">"T"&amp;M149&amp;B149</f>
+        <f t="shared" ref="H149:H183" si="89">"T"&amp;M149&amp;B149</f>
         <v>TTMDBWatchProvider</v>
       </c>
       <c r="I149" s="8" t="str">
@@ -12411,11 +12417,11 @@
         <v xml:space="preserve">  TTMDBWatchProvider = class;</v>
       </c>
       <c r="K149" s="8" t="str">
-        <f t="shared" ref="K149:K181" si="90">IF(C149="", "  "&amp;G149&amp;" = interface", "  "&amp;G149&amp;" = interface(I"&amp;M149&amp;C149&amp;")")</f>
+        <f t="shared" ref="K149:K183" si="90">IF(C149="", "  "&amp;G149&amp;" = interface", "  "&amp;G149&amp;" = interface(I"&amp;M149&amp;C149&amp;")")</f>
         <v xml:space="preserve">  ITMDBWatchProvider = interface(ITMDBItem)</v>
       </c>
       <c r="L149" s="8" t="str">
-        <f t="shared" ref="L149:L181" si="91">IF(C149="", "  "&amp;H149&amp;" = class(TInterfacedObject, "&amp;G149&amp;")", "  "&amp;H149&amp;" = class(T"&amp;M149&amp;C149&amp;", "&amp;G149&amp;")")</f>
+        <f t="shared" ref="L149:L183" si="91">IF(C149="", "  "&amp;H149&amp;" = class(TInterfacedObject, "&amp;G149&amp;")", "  "&amp;H149&amp;" = class(T"&amp;M149&amp;C149&amp;", "&amp;G149&amp;")")</f>
         <v xml:space="preserve">  TTMDBWatchProvider = class(TTMDBItem, ITMDBWatchProvider)</v>
       </c>
       <c r="M149" s="8" t="s">
@@ -12474,16 +12480,16 @@
         <v>150</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C151" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="D151" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E151" s="12" t="s">
-        <v>74</v>
+      <c r="D151" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E151" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="F151" s="12" t="s">
         <v>74</v>
@@ -12521,16 +12527,16 @@
         <v>150</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C152" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="D152" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E152" s="12" t="s">
-        <v>74</v>
+      <c r="D152" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E152" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="F152" s="12" t="s">
         <v>74</v>
@@ -12565,10 +12571,10 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="10" t="s">
-        <v>388</v>
+        <v>150</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="D153" s="14" t="s">
         <v>377</v>
@@ -12576,32 +12582,32 @@
       <c r="E153" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F153" s="14" t="s">
-        <v>377</v>
+      <c r="F153" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G153" s="8" t="str">
-        <f t="shared" si="88"/>
-        <v>ITMDBNamespace</v>
+        <f t="shared" ref="G153" si="98">"I"&amp;M153&amp;B153</f>
+        <v>ITMDBMediaWatchProviderCountry</v>
       </c>
       <c r="H153" s="8" t="str">
-        <f t="shared" si="89"/>
-        <v>TTMDBNamespace</v>
+        <f t="shared" ref="H153" si="99">"T"&amp;M153&amp;B153</f>
+        <v>TTMDBMediaWatchProviderCountry</v>
       </c>
       <c r="I153" s="8" t="str">
-        <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespace = interface;</v>
+        <f t="shared" ref="I153" si="100">"  "&amp;G153&amp;" = interface;"</f>
+        <v xml:space="preserve">  ITMDBMediaWatchProviderCountry = interface;</v>
       </c>
       <c r="J153" s="8" t="str">
-        <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespace = class;</v>
+        <f t="shared" ref="J153" si="101">"  "&amp;H153&amp;" = class;"</f>
+        <v xml:space="preserve">  TTMDBMediaWatchProviderCountry = class;</v>
       </c>
       <c r="K153" s="8" t="str">
-        <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespace = interface</v>
+        <f t="shared" ref="K153" si="102">IF(C153="", "  "&amp;G153&amp;" = interface", "  "&amp;G153&amp;" = interface(I"&amp;M153&amp;C153&amp;")")</f>
+        <v xml:space="preserve">  ITMDBMediaWatchProviderCountry = interface</v>
       </c>
       <c r="L153" s="8" t="str">
-        <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespace = class(TInterfacedObject, ITMDBNamespace)</v>
+        <f t="shared" ref="L153" si="103">IF(C153="", "  "&amp;H153&amp;" = class(TInterfacedObject, "&amp;G153&amp;")", "  "&amp;H153&amp;" = class(T"&amp;M153&amp;C153&amp;", "&amp;G153&amp;")")</f>
+        <v xml:space="preserve">  TTMDBMediaWatchProviderCountry = class(TInterfacedObject, ITMDBMediaWatchProviderCountry)</v>
       </c>
       <c r="M153" s="8" t="s">
         <v>259</v>
@@ -12609,13 +12615,10 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="10" t="s">
-        <v>388</v>
+        <v>150</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="C154" s="10" t="s">
-        <v>390</v>
+        <v>489</v>
       </c>
       <c r="D154" s="14" t="s">
         <v>377</v>
@@ -12623,32 +12626,32 @@
       <c r="E154" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F154" s="13" t="s">
-        <v>255</v>
+      <c r="F154" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G154" s="8" t="str">
-        <f t="shared" si="88"/>
-        <v>ITMDBNamespaceAccount</v>
+        <f t="shared" ref="G154" si="104">"I"&amp;M154&amp;B154</f>
+        <v>ITMDBMediaWatchProviderCountries</v>
       </c>
       <c r="H154" s="8" t="str">
-        <f t="shared" si="89"/>
-        <v>TTMDBNamespaceAccount</v>
+        <f t="shared" ref="H154" si="105">"T"&amp;M154&amp;B154</f>
+        <v>TTMDBMediaWatchProviderCountries</v>
       </c>
       <c r="I154" s="8" t="str">
-        <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceAccount = interface;</v>
+        <f t="shared" ref="I154" si="106">"  "&amp;G154&amp;" = interface;"</f>
+        <v xml:space="preserve">  ITMDBMediaWatchProviderCountries = interface;</v>
       </c>
       <c r="J154" s="8" t="str">
-        <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceAccount = class;</v>
+        <f t="shared" ref="J154" si="107">"  "&amp;H154&amp;" = class;"</f>
+        <v xml:space="preserve">  TTMDBMediaWatchProviderCountries = class;</v>
       </c>
       <c r="K154" s="8" t="str">
-        <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceAccount = interface(ITMDBITMDBNamespace)</v>
+        <f t="shared" ref="K154" si="108">IF(C154="", "  "&amp;G154&amp;" = interface", "  "&amp;G154&amp;" = interface(I"&amp;M154&amp;C154&amp;")")</f>
+        <v xml:space="preserve">  ITMDBMediaWatchProviderCountries = interface</v>
       </c>
       <c r="L154" s="8" t="str">
-        <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceAccount = class(TTMDBITMDBNamespace, ITMDBNamespaceAccount)</v>
+        <f t="shared" ref="L154" si="109">IF(C154="", "  "&amp;H154&amp;" = class(TInterfacedObject, "&amp;G154&amp;")", "  "&amp;H154&amp;" = class(T"&amp;M154&amp;C154&amp;", "&amp;G154&amp;")")</f>
+        <v xml:space="preserve">  TTMDBMediaWatchProviderCountries = class(TInterfacedObject, ITMDBMediaWatchProviderCountries)</v>
       </c>
       <c r="M154" s="8" t="s">
         <v>259</v>
@@ -12659,10 +12662,7 @@
         <v>388</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="C155" s="10" t="s">
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="D155" s="14" t="s">
         <v>377</v>
@@ -12670,32 +12670,32 @@
       <c r="E155" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F155" s="13" t="s">
-        <v>255</v>
+      <c r="F155" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="G155" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceAuthentication</v>
+        <v>ITMDBNamespace</v>
       </c>
       <c r="H155" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceAuthentication</v>
+        <v>TTMDBNamespace</v>
       </c>
       <c r="I155" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceAuthentication = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespace = interface;</v>
       </c>
       <c r="J155" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceAuthentication = class;</v>
+        <v xml:space="preserve">  TTMDBNamespace = class;</v>
       </c>
       <c r="K155" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceAuthentication = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespace = interface</v>
       </c>
       <c r="L155" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceAuthentication = class(TTMDBITMDBNamespace, ITMDBNamespaceAuthentication)</v>
+        <v xml:space="preserve">  TTMDBNamespace = class(TInterfacedObject, ITMDBNamespace)</v>
       </c>
       <c r="M155" s="8" t="s">
         <v>259</v>
@@ -12706,7 +12706,7 @@
         <v>388</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C156" s="10" t="s">
         <v>390</v>
@@ -12717,32 +12717,32 @@
       <c r="E156" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F156" s="14" t="s">
-        <v>377</v>
+      <c r="F156" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="G156" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceCertifications</v>
+        <v>ITMDBNamespaceAccount</v>
       </c>
       <c r="H156" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceCertifications</v>
+        <v>TTMDBNamespaceAccount</v>
       </c>
       <c r="I156" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceCertifications = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceAccount = interface;</v>
       </c>
       <c r="J156" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceCertifications = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceAccount = class;</v>
       </c>
       <c r="K156" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceCertifications = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceAccount = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L156" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceCertifications = class(TTMDBITMDBNamespace, ITMDBNamespaceCertifications)</v>
+        <v xml:space="preserve">  TTMDBNamespaceAccount = class(TTMDBITMDBNamespace, ITMDBNamespaceAccount)</v>
       </c>
       <c r="M156" s="8" t="s">
         <v>259</v>
@@ -12753,7 +12753,7 @@
         <v>388</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C157" s="10" t="s">
         <v>390</v>
@@ -12764,32 +12764,32 @@
       <c r="E157" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F157" s="12" t="s">
-        <v>74</v>
+      <c r="F157" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="G157" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceChanges</v>
+        <v>ITMDBNamespaceAuthentication</v>
       </c>
       <c r="H157" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceChanges</v>
+        <v>TTMDBNamespaceAuthentication</v>
       </c>
       <c r="I157" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceChanges = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceAuthentication = interface;</v>
       </c>
       <c r="J157" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceChanges = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceAuthentication = class;</v>
       </c>
       <c r="K157" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceChanges = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceAuthentication = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L157" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceChanges = class(TTMDBITMDBNamespace, ITMDBNamespaceChanges)</v>
+        <v xml:space="preserve">  TTMDBNamespaceAuthentication = class(TTMDBITMDBNamespace, ITMDBNamespaceAuthentication)</v>
       </c>
       <c r="M157" s="8" t="s">
         <v>259</v>
@@ -12800,7 +12800,7 @@
         <v>388</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C158" s="10" t="s">
         <v>390</v>
@@ -12811,32 +12811,32 @@
       <c r="E158" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F158" s="13" t="s">
-        <v>255</v>
+      <c r="F158" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="G158" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceCollections</v>
+        <v>ITMDBNamespaceCertifications</v>
       </c>
       <c r="H158" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceCollections</v>
+        <v>TTMDBNamespaceCertifications</v>
       </c>
       <c r="I158" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceCollections = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceCertifications = interface;</v>
       </c>
       <c r="J158" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceCollections = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceCertifications = class;</v>
       </c>
       <c r="K158" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceCollections = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceCertifications = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L158" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceCollections = class(TTMDBITMDBNamespace, ITMDBNamespaceCollections)</v>
+        <v xml:space="preserve">  TTMDBNamespaceCertifications = class(TTMDBITMDBNamespace, ITMDBNamespaceCertifications)</v>
       </c>
       <c r="M158" s="8" t="s">
         <v>259</v>
@@ -12847,7 +12847,7 @@
         <v>388</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>390</v>
@@ -12858,32 +12858,32 @@
       <c r="E159" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F159" s="13" t="s">
-        <v>255</v>
+      <c r="F159" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G159" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceCompanies</v>
+        <v>ITMDBNamespaceChanges</v>
       </c>
       <c r="H159" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceCompanies</v>
+        <v>TTMDBNamespaceChanges</v>
       </c>
       <c r="I159" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceCompanies = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceChanges = interface;</v>
       </c>
       <c r="J159" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceCompanies = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceChanges = class;</v>
       </c>
       <c r="K159" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceCompanies = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceChanges = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L159" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceCompanies = class(TTMDBITMDBNamespace, ITMDBNamespaceCompanies)</v>
+        <v xml:space="preserve">  TTMDBNamespaceChanges = class(TTMDBITMDBNamespace, ITMDBNamespaceChanges)</v>
       </c>
       <c r="M159" s="8" t="s">
         <v>259</v>
@@ -12894,7 +12894,7 @@
         <v>388</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C160" s="10" t="s">
         <v>390</v>
@@ -12905,32 +12905,32 @@
       <c r="E160" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F160" s="15" t="s">
-        <v>256</v>
+      <c r="F160" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="G160" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceConfiguration</v>
+        <v>ITMDBNamespaceCollections</v>
       </c>
       <c r="H160" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceConfiguration</v>
+        <v>TTMDBNamespaceCollections</v>
       </c>
       <c r="I160" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceConfiguration = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceCollections = interface;</v>
       </c>
       <c r="J160" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceConfiguration = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceCollections = class;</v>
       </c>
       <c r="K160" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceConfiguration = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceCollections = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L160" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceConfiguration = class(TTMDBITMDBNamespace, ITMDBNamespaceConfiguration)</v>
+        <v xml:space="preserve">  TTMDBNamespaceCollections = class(TTMDBITMDBNamespace, ITMDBNamespaceCollections)</v>
       </c>
       <c r="M160" s="8" t="s">
         <v>259</v>
@@ -12941,7 +12941,7 @@
         <v>388</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C161" s="10" t="s">
         <v>390</v>
@@ -12952,32 +12952,32 @@
       <c r="E161" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F161" s="12" t="s">
-        <v>74</v>
+      <c r="F161" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="G161" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceCredits</v>
+        <v>ITMDBNamespaceCompanies</v>
       </c>
       <c r="H161" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceCredits</v>
+        <v>TTMDBNamespaceCompanies</v>
       </c>
       <c r="I161" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceCredits = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceCompanies = interface;</v>
       </c>
       <c r="J161" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceCredits = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceCompanies = class;</v>
       </c>
       <c r="K161" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceCredits = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceCompanies = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L161" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceCredits = class(TTMDBITMDBNamespace, ITMDBNamespaceCredits)</v>
+        <v xml:space="preserve">  TTMDBNamespaceCompanies = class(TTMDBITMDBNamespace, ITMDBNamespaceCompanies)</v>
       </c>
       <c r="M161" s="8" t="s">
         <v>259</v>
@@ -12988,7 +12988,7 @@
         <v>388</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C162" s="10" t="s">
         <v>390</v>
@@ -12999,32 +12999,32 @@
       <c r="E162" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F162" s="12" t="s">
-        <v>74</v>
+      <c r="F162" s="15" t="s">
+        <v>256</v>
       </c>
       <c r="G162" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceDiscover</v>
+        <v>ITMDBNamespaceConfiguration</v>
       </c>
       <c r="H162" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceDiscover</v>
+        <v>TTMDBNamespaceConfiguration</v>
       </c>
       <c r="I162" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceDiscover = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceConfiguration = interface;</v>
       </c>
       <c r="J162" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceDiscover = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceConfiguration = class;</v>
       </c>
       <c r="K162" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceDiscover = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceConfiguration = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L162" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceDiscover = class(TTMDBITMDBNamespace, ITMDBNamespaceDiscover)</v>
+        <v xml:space="preserve">  TTMDBNamespaceConfiguration = class(TTMDBITMDBNamespace, ITMDBNamespaceConfiguration)</v>
       </c>
       <c r="M162" s="8" t="s">
         <v>259</v>
@@ -13035,7 +13035,7 @@
         <v>388</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C163" s="10" t="s">
         <v>390</v>
@@ -13051,27 +13051,27 @@
       </c>
       <c r="G163" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceFind</v>
+        <v>ITMDBNamespaceCredits</v>
       </c>
       <c r="H163" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceFind</v>
+        <v>TTMDBNamespaceCredits</v>
       </c>
       <c r="I163" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceFind = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceCredits = interface;</v>
       </c>
       <c r="J163" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceFind = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceCredits = class;</v>
       </c>
       <c r="K163" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceFind = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceCredits = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L163" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceFind = class(TTMDBITMDBNamespace, ITMDBNamespaceFind)</v>
+        <v xml:space="preserve">  TTMDBNamespaceCredits = class(TTMDBITMDBNamespace, ITMDBNamespaceCredits)</v>
       </c>
       <c r="M163" s="8" t="s">
         <v>259</v>
@@ -13082,7 +13082,7 @@
         <v>388</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C164" s="10" t="s">
         <v>390</v>
@@ -13093,32 +13093,32 @@
       <c r="E164" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F164" s="14" t="s">
-        <v>377</v>
+      <c r="F164" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G164" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceGenres</v>
+        <v>ITMDBNamespaceDiscover</v>
       </c>
       <c r="H164" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceGenres</v>
+        <v>TTMDBNamespaceDiscover</v>
       </c>
       <c r="I164" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceGenres = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceDiscover = interface;</v>
       </c>
       <c r="J164" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceGenres = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceDiscover = class;</v>
       </c>
       <c r="K164" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceGenres = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceDiscover = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L164" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceGenres = class(TTMDBITMDBNamespace, ITMDBNamespaceGenres)</v>
+        <v xml:space="preserve">  TTMDBNamespaceDiscover = class(TTMDBITMDBNamespace, ITMDBNamespaceDiscover)</v>
       </c>
       <c r="M164" s="8" t="s">
         <v>259</v>
@@ -13129,7 +13129,7 @@
         <v>388</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C165" s="10" t="s">
         <v>390</v>
@@ -13145,27 +13145,27 @@
       </c>
       <c r="G165" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceGuestSessions</v>
+        <v>ITMDBNamespaceFind</v>
       </c>
       <c r="H165" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceGuestSessions</v>
+        <v>TTMDBNamespaceFind</v>
       </c>
       <c r="I165" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceGuestSessions = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceFind = interface;</v>
       </c>
       <c r="J165" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceGuestSessions = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceFind = class;</v>
       </c>
       <c r="K165" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceGuestSessions = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceFind = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L165" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceGuestSessions = class(TTMDBITMDBNamespace, ITMDBNamespaceGuestSessions)</v>
+        <v xml:space="preserve">  TTMDBNamespaceFind = class(TTMDBITMDBNamespace, ITMDBNamespaceFind)</v>
       </c>
       <c r="M165" s="8" t="s">
         <v>259</v>
@@ -13176,7 +13176,7 @@
         <v>388</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C166" s="10" t="s">
         <v>390</v>
@@ -13192,27 +13192,27 @@
       </c>
       <c r="G166" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceKeywords</v>
+        <v>ITMDBNamespaceGenres</v>
       </c>
       <c r="H166" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceKeywords</v>
+        <v>TTMDBNamespaceGenres</v>
       </c>
       <c r="I166" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceKeywords = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceGenres = interface;</v>
       </c>
       <c r="J166" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceKeywords = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceGenres = class;</v>
       </c>
       <c r="K166" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceKeywords = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceGenres = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L166" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceKeywords = class(TTMDBITMDBNamespace, ITMDBNamespaceKeywords)</v>
+        <v xml:space="preserve">  TTMDBNamespaceGenres = class(TTMDBITMDBNamespace, ITMDBNamespaceGenres)</v>
       </c>
       <c r="M166" s="8" t="s">
         <v>259</v>
@@ -13223,43 +13223,43 @@
         <v>388</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C167" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D167" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E167" s="12" t="s">
-        <v>74</v>
+      <c r="D167" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E167" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="F167" s="12" t="s">
         <v>74</v>
       </c>
       <c r="G167" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceLists</v>
+        <v>ITMDBNamespaceGuestSessions</v>
       </c>
       <c r="H167" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceLists</v>
+        <v>TTMDBNamespaceGuestSessions</v>
       </c>
       <c r="I167" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceLists = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceGuestSessions = interface;</v>
       </c>
       <c r="J167" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceLists = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceGuestSessions = class;</v>
       </c>
       <c r="K167" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceLists = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceGuestSessions = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L167" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceLists = class(TTMDBITMDBNamespace, ITMDBNamespaceLists)</v>
+        <v xml:space="preserve">  TTMDBNamespaceGuestSessions = class(TTMDBITMDBNamespace, ITMDBNamespaceGuestSessions)</v>
       </c>
       <c r="M167" s="8" t="s">
         <v>259</v>
@@ -13270,7 +13270,7 @@
         <v>388</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C168" s="10" t="s">
         <v>390</v>
@@ -13281,32 +13281,32 @@
       <c r="E168" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F168" s="12" t="s">
-        <v>74</v>
+      <c r="F168" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="G168" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceMovieLists</v>
+        <v>ITMDBNamespaceKeywords</v>
       </c>
       <c r="H168" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceMovieLists</v>
+        <v>TTMDBNamespaceKeywords</v>
       </c>
       <c r="I168" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceMovieLists = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceKeywords = interface;</v>
       </c>
       <c r="J168" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceMovieLists = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceKeywords = class;</v>
       </c>
       <c r="K168" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceMovieLists = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceKeywords = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L168" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceMovieLists = class(TTMDBITMDBNamespace, ITMDBNamespaceMovieLists)</v>
+        <v xml:space="preserve">  TTMDBNamespaceKeywords = class(TTMDBITMDBNamespace, ITMDBNamespaceKeywords)</v>
       </c>
       <c r="M168" s="8" t="s">
         <v>259</v>
@@ -13317,43 +13317,43 @@
         <v>388</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C169" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D169" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E169" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F169" s="15" t="s">
-        <v>256</v>
+      <c r="D169" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F169" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G169" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceMovies</v>
+        <v>ITMDBNamespaceLists</v>
       </c>
       <c r="H169" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceMovies</v>
+        <v>TTMDBNamespaceLists</v>
       </c>
       <c r="I169" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceMovies = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceLists = interface;</v>
       </c>
       <c r="J169" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceMovies = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceLists = class;</v>
       </c>
       <c r="K169" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceMovies = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceLists = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L169" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceMovies = class(TTMDBITMDBNamespace, ITMDBNamespaceMovies)</v>
+        <v xml:space="preserve">  TTMDBNamespaceLists = class(TTMDBITMDBNamespace, ITMDBNamespaceLists)</v>
       </c>
       <c r="M169" s="8" t="s">
         <v>259</v>
@@ -13364,7 +13364,7 @@
         <v>388</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C170" s="10" t="s">
         <v>390</v>
@@ -13375,32 +13375,32 @@
       <c r="E170" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F170" s="15" t="s">
-        <v>256</v>
+      <c r="F170" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G170" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceNetworks</v>
+        <v>ITMDBNamespaceMovieLists</v>
       </c>
       <c r="H170" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceNetworks</v>
+        <v>TTMDBNamespaceMovieLists</v>
       </c>
       <c r="I170" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceNetworks = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceMovieLists = interface;</v>
       </c>
       <c r="J170" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceNetworks = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceMovieLists = class;</v>
       </c>
       <c r="K170" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceNetworks = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceMovieLists = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L170" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceNetworks = class(TTMDBITMDBNamespace, ITMDBNamespaceNetworks)</v>
+        <v xml:space="preserve">  TTMDBNamespaceMovieLists = class(TTMDBITMDBNamespace, ITMDBNamespaceMovieLists)</v>
       </c>
       <c r="M170" s="8" t="s">
         <v>259</v>
@@ -13411,43 +13411,43 @@
         <v>388</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C171" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D171" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="E171" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="F171" s="12" t="s">
-        <v>74</v>
+      <c r="D171" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E171" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F171" s="15" t="s">
+        <v>256</v>
       </c>
       <c r="G171" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespacePeopleLists</v>
+        <v>ITMDBNamespaceMovies</v>
       </c>
       <c r="H171" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespacePeopleLists</v>
+        <v>TTMDBNamespaceMovies</v>
       </c>
       <c r="I171" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespacePeopleLists = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceMovies = interface;</v>
       </c>
       <c r="J171" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespacePeopleLists = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceMovies = class;</v>
       </c>
       <c r="K171" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespacePeopleLists = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceMovies = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L171" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespacePeopleLists = class(TTMDBITMDBNamespace, ITMDBNamespacePeopleLists)</v>
+        <v xml:space="preserve">  TTMDBNamespaceMovies = class(TTMDBITMDBNamespace, ITMDBNamespaceMovies)</v>
       </c>
       <c r="M171" s="8" t="s">
         <v>259</v>
@@ -13458,43 +13458,43 @@
         <v>388</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C172" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D172" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E172" s="15" t="s">
-        <v>256</v>
+      <c r="D172" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E172" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="F172" s="15" t="s">
         <v>256</v>
       </c>
       <c r="G172" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespacePeople</v>
+        <v>ITMDBNamespaceNetworks</v>
       </c>
       <c r="H172" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespacePeople</v>
+        <v>TTMDBNamespaceNetworks</v>
       </c>
       <c r="I172" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespacePeople = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceNetworks = interface;</v>
       </c>
       <c r="J172" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespacePeople = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceNetworks = class;</v>
       </c>
       <c r="K172" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespacePeople = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceNetworks = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L172" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespacePeople = class(TTMDBITMDBNamespace, ITMDBNamespacePeople)</v>
+        <v xml:space="preserve">  TTMDBNamespaceNetworks = class(TTMDBITMDBNamespace, ITMDBNamespaceNetworks)</v>
       </c>
       <c r="M172" s="8" t="s">
         <v>259</v>
@@ -13505,7 +13505,7 @@
         <v>388</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C173" s="10" t="s">
         <v>390</v>
@@ -13521,27 +13521,27 @@
       </c>
       <c r="G173" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceReviews</v>
+        <v>ITMDBNamespacePeopleLists</v>
       </c>
       <c r="H173" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceReviews</v>
+        <v>TTMDBNamespacePeopleLists</v>
       </c>
       <c r="I173" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceReviews = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespacePeopleLists = interface;</v>
       </c>
       <c r="J173" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceReviews = class;</v>
+        <v xml:space="preserve">  TTMDBNamespacePeopleLists = class;</v>
       </c>
       <c r="K173" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceReviews = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespacePeopleLists = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L173" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceReviews = class(TTMDBITMDBNamespace, ITMDBNamespaceReviews)</v>
+        <v xml:space="preserve">  TTMDBNamespacePeopleLists = class(TTMDBITMDBNamespace, ITMDBNamespacePeopleLists)</v>
       </c>
       <c r="M173" s="8" t="s">
         <v>259</v>
@@ -13552,43 +13552,43 @@
         <v>388</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C174" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D174" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="E174" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="F174" s="13" t="s">
-        <v>255</v>
+      <c r="D174" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E174" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F174" s="15" t="s">
+        <v>256</v>
       </c>
       <c r="G174" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceSearch</v>
+        <v>ITMDBNamespacePeople</v>
       </c>
       <c r="H174" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceSearch</v>
+        <v>TTMDBNamespacePeople</v>
       </c>
       <c r="I174" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceSearch = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespacePeople = interface;</v>
       </c>
       <c r="J174" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceSearch = class;</v>
+        <v xml:space="preserve">  TTMDBNamespacePeople = class;</v>
       </c>
       <c r="K174" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceSearch = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespacePeople = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L174" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceSearch = class(TTMDBITMDBNamespace, ITMDBNamespaceSearch)</v>
+        <v xml:space="preserve">  TTMDBNamespacePeople = class(TTMDBITMDBNamespace, ITMDBNamespacePeople)</v>
       </c>
       <c r="M174" s="8" t="s">
         <v>259</v>
@@ -13599,7 +13599,7 @@
         <v>388</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C175" s="10" t="s">
         <v>390</v>
@@ -13615,27 +13615,27 @@
       </c>
       <c r="G175" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTrending</v>
+        <v>ITMDBNamespaceReviews</v>
       </c>
       <c r="H175" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTrending</v>
+        <v>TTMDBNamespaceReviews</v>
       </c>
       <c r="I175" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTrending = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceReviews = interface;</v>
       </c>
       <c r="J175" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTrending = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceReviews = class;</v>
       </c>
       <c r="K175" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTrending = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceReviews = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L175" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTrending = class(TTMDBITMDBNamespace, ITMDBNamespaceTrending)</v>
+        <v xml:space="preserve">  TTMDBNamespaceReviews = class(TTMDBITMDBNamespace, ITMDBNamespaceReviews)</v>
       </c>
       <c r="M175" s="8" t="s">
         <v>259</v>
@@ -13646,7 +13646,7 @@
         <v>388</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C176" s="10" t="s">
         <v>390</v>
@@ -13657,32 +13657,32 @@
       <c r="E176" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F176" s="12" t="s">
-        <v>74</v>
+      <c r="F176" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="G176" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTVSeriesLists</v>
+        <v>ITMDBNamespaceSearch</v>
       </c>
       <c r="H176" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTVSeriesLists</v>
+        <v>TTMDBNamespaceSearch</v>
       </c>
       <c r="I176" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeriesLists = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceSearch = interface;</v>
       </c>
       <c r="J176" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeriesLists = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceSearch = class;</v>
       </c>
       <c r="K176" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeriesLists = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceSearch = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L176" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeriesLists = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeriesLists)</v>
+        <v xml:space="preserve">  TTMDBNamespaceSearch = class(TTMDBITMDBNamespace, ITMDBNamespaceSearch)</v>
       </c>
       <c r="M176" s="8" t="s">
         <v>259</v>
@@ -13693,43 +13693,43 @@
         <v>388</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C177" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D177" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E177" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F177" s="15" t="s">
-        <v>256</v>
+      <c r="D177" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E177" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="F177" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G177" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTVSeries</v>
+        <v>ITMDBNamespaceTrending</v>
       </c>
       <c r="H177" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTVSeries</v>
+        <v>TTMDBNamespaceTrending</v>
       </c>
       <c r="I177" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeries = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTrending = interface;</v>
       </c>
       <c r="J177" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeries = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTrending = class;</v>
       </c>
       <c r="K177" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeries = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceTrending = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L177" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeries = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeries)</v>
+        <v xml:space="preserve">  TTMDBNamespaceTrending = class(TTMDBITMDBNamespace, ITMDBNamespaceTrending)</v>
       </c>
       <c r="M177" s="8" t="s">
         <v>259</v>
@@ -13740,43 +13740,43 @@
         <v>388</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C178" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D178" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E178" s="15" t="s">
-        <v>256</v>
+      <c r="D178" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E178" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="F178" s="12" t="s">
         <v>74</v>
       </c>
       <c r="G178" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTVSeasons</v>
+        <v>ITMDBNamespaceTVSeriesLists</v>
       </c>
       <c r="H178" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTVSeasons</v>
+        <v>TTMDBNamespaceTVSeriesLists</v>
       </c>
       <c r="I178" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeasons = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeriesLists = interface;</v>
       </c>
       <c r="J178" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeasons = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeriesLists = class;</v>
       </c>
       <c r="K178" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVSeasons = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeriesLists = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L178" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVSeasons = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeasons)</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeriesLists = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeriesLists)</v>
       </c>
       <c r="M178" s="8" t="s">
         <v>259</v>
@@ -13787,7 +13787,7 @@
         <v>388</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C179" s="10" t="s">
         <v>390</v>
@@ -13798,32 +13798,32 @@
       <c r="E179" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="F179" s="12" t="s">
-        <v>74</v>
+      <c r="F179" s="15" t="s">
+        <v>256</v>
       </c>
       <c r="G179" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTVEpisodes</v>
+        <v>ITMDBNamespaceTVSeries</v>
       </c>
       <c r="H179" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTVEpisodes</v>
+        <v>TTMDBNamespaceTVSeries</v>
       </c>
       <c r="I179" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVEpisodes = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeries = interface;</v>
       </c>
       <c r="J179" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVEpisodes = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeries = class;</v>
       </c>
       <c r="K179" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVEpisodes = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeries = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L179" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVEpisodes = class(TTMDBITMDBNamespace, ITMDBNamespaceTVEpisodes)</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeries = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeries)</v>
       </c>
       <c r="M179" s="8" t="s">
         <v>259</v>
@@ -13834,7 +13834,7 @@
         <v>388</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C180" s="10" t="s">
         <v>390</v>
@@ -13850,27 +13850,27 @@
       </c>
       <c r="G180" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceTVEpisodeGroups</v>
+        <v>ITMDBNamespaceTVSeasons</v>
       </c>
       <c r="H180" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceTVEpisodeGroups</v>
+        <v>TTMDBNamespaceTVSeasons</v>
       </c>
       <c r="I180" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVEpisodeGroups = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeasons = interface;</v>
       </c>
       <c r="J180" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVEpisodeGroups = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeasons = class;</v>
       </c>
       <c r="K180" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceTVEpisodeGroups = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVSeasons = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L180" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceTVEpisodeGroups = class(TTMDBITMDBNamespace, ITMDBNamespaceTVEpisodeGroups)</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVSeasons = class(TTMDBITMDBNamespace, ITMDBNamespaceTVSeasons)</v>
       </c>
       <c r="M180" s="8" t="s">
         <v>259</v>
@@ -13881,43 +13881,43 @@
         <v>388</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C181" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D181" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="E181" s="14" t="s">
-        <v>377</v>
+      <c r="D181" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E181" s="15" t="s">
+        <v>256</v>
       </c>
       <c r="F181" s="12" t="s">
         <v>74</v>
       </c>
       <c r="G181" s="8" t="str">
         <f t="shared" si="88"/>
-        <v>ITMDBNamespaceWatchProviders</v>
+        <v>ITMDBNamespaceTVEpisodes</v>
       </c>
       <c r="H181" s="8" t="str">
         <f t="shared" si="89"/>
-        <v>TTMDBNamespaceWatchProviders</v>
+        <v>TTMDBNamespaceTVEpisodes</v>
       </c>
       <c r="I181" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBNamespaceWatchProviders = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVEpisodes = interface;</v>
       </c>
       <c r="J181" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBNamespaceWatchProviders = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVEpisodes = class;</v>
       </c>
       <c r="K181" s="8" t="str">
         <f t="shared" si="90"/>
-        <v xml:space="preserve">  ITMDBNamespaceWatchProviders = interface(ITMDBITMDBNamespace)</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVEpisodes = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L181" s="8" t="str">
         <f t="shared" si="91"/>
-        <v xml:space="preserve">  TTMDBNamespaceWatchProviders = class(TTMDBITMDBNamespace, ITMDBNamespaceWatchProviders)</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVEpisodes = class(TTMDBITMDBNamespace, ITMDBNamespaceTVEpisodes)</v>
       </c>
       <c r="M181" s="8" t="s">
         <v>259</v>
@@ -13925,10 +13925,13 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
-        <v>372</v>
+        <v>388</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>366</v>
+        <v>416</v>
+      </c>
+      <c r="C182" s="10" t="s">
+        <v>390</v>
       </c>
       <c r="D182" s="14" t="s">
         <v>377</v>
@@ -13936,32 +13939,32 @@
       <c r="E182" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F182" s="13" t="s">
-        <v>255</v>
+      <c r="F182" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G182" s="8" t="str">
-        <f t="shared" ref="G182:G186" si="98">"I"&amp;M182&amp;B182</f>
-        <v>ITMDBCache</v>
+        <f t="shared" si="88"/>
+        <v>ITMDBNamespaceTVEpisodeGroups</v>
       </c>
       <c r="H182" s="8" t="str">
-        <f t="shared" ref="H182:H186" si="99">"T"&amp;M182&amp;B182</f>
-        <v>TTMDBCache</v>
+        <f t="shared" si="89"/>
+        <v>TTMDBNamespaceTVEpisodeGroups</v>
       </c>
       <c r="I182" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBCache = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceTVEpisodeGroups = interface;</v>
       </c>
       <c r="J182" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBCache = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceTVEpisodeGroups = class;</v>
       </c>
       <c r="K182" s="8" t="str">
-        <f t="shared" ref="K182:K186" si="100">IF(C182="", "  "&amp;G182&amp;" = interface", "  "&amp;G182&amp;" = interface(I"&amp;M182&amp;C182&amp;")")</f>
-        <v xml:space="preserve">  ITMDBCache = interface</v>
+        <f t="shared" si="90"/>
+        <v xml:space="preserve">  ITMDBNamespaceTVEpisodeGroups = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L182" s="8" t="str">
-        <f t="shared" ref="L182:L186" si="101">IF(C182="", "  "&amp;H182&amp;" = class(TInterfacedObject, "&amp;G182&amp;")", "  "&amp;H182&amp;" = class(T"&amp;M182&amp;C182&amp;", "&amp;G182&amp;")")</f>
-        <v xml:space="preserve">  TTMDBCache = class(TInterfacedObject, ITMDBCache)</v>
+        <f t="shared" si="91"/>
+        <v xml:space="preserve">  TTMDBNamespaceTVEpisodeGroups = class(TTMDBITMDBNamespace, ITMDBNamespaceTVEpisodeGroups)</v>
       </c>
       <c r="M182" s="8" t="s">
         <v>259</v>
@@ -13969,10 +13972,13 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="10" t="s">
-        <v>372</v>
+        <v>388</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>367</v>
+        <v>417</v>
+      </c>
+      <c r="C183" s="10" t="s">
+        <v>390</v>
       </c>
       <c r="D183" s="14" t="s">
         <v>377</v>
@@ -13980,32 +13986,32 @@
       <c r="E183" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F183" s="13" t="s">
-        <v>255</v>
+      <c r="F183" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G183" s="8" t="str">
-        <f t="shared" si="98"/>
-        <v>ITMDBLoginState</v>
+        <f t="shared" si="88"/>
+        <v>ITMDBNamespaceWatchProviders</v>
       </c>
       <c r="H183" s="8" t="str">
-        <f t="shared" si="99"/>
-        <v>TTMDBLoginState</v>
+        <f t="shared" si="89"/>
+        <v>TTMDBNamespaceWatchProviders</v>
       </c>
       <c r="I183" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBLoginState = interface;</v>
+        <v xml:space="preserve">  ITMDBNamespaceWatchProviders = interface;</v>
       </c>
       <c r="J183" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBLoginState = class;</v>
+        <v xml:space="preserve">  TTMDBNamespaceWatchProviders = class;</v>
       </c>
       <c r="K183" s="8" t="str">
-        <f t="shared" si="100"/>
-        <v xml:space="preserve">  ITMDBLoginState = interface</v>
+        <f t="shared" si="90"/>
+        <v xml:space="preserve">  ITMDBNamespaceWatchProviders = interface(ITMDBITMDBNamespace)</v>
       </c>
       <c r="L183" s="8" t="str">
-        <f t="shared" si="101"/>
-        <v xml:space="preserve">  TTMDBLoginState = class(TInterfacedObject, ITMDBLoginState)</v>
+        <f t="shared" si="91"/>
+        <v xml:space="preserve">  TTMDBNamespaceWatchProviders = class(TTMDBITMDBNamespace, ITMDBNamespaceWatchProviders)</v>
       </c>
       <c r="M183" s="8" t="s">
         <v>259</v>
@@ -14016,7 +14022,7 @@
         <v>372</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D184" s="14" t="s">
         <v>377</v>
@@ -14024,92 +14030,180 @@
       <c r="E184" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F184" s="13" t="s">
-        <v>255</v>
+      <c r="F184" s="14" t="s">
+        <v>377</v>
       </c>
       <c r="G184" s="8" t="str">
-        <f t="shared" si="98"/>
-        <v>ITMDBClient</v>
+        <f t="shared" ref="G184:G188" si="110">"I"&amp;M184&amp;B184</f>
+        <v>ITMDBCache</v>
       </c>
       <c r="H184" s="8" t="str">
-        <f t="shared" si="99"/>
-        <v>TTMDBClient</v>
+        <f t="shared" ref="H184:H188" si="111">"T"&amp;M184&amp;B184</f>
+        <v>TTMDBCache</v>
       </c>
       <c r="I184" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDBClient = interface;</v>
+        <v xml:space="preserve">  ITMDBCache = interface;</v>
       </c>
       <c r="J184" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDBClient = class;</v>
+        <v xml:space="preserve">  TTMDBCache = class;</v>
       </c>
       <c r="K184" s="8" t="str">
-        <f t="shared" si="100"/>
-        <v xml:space="preserve">  ITMDBClient = interface</v>
+        <f t="shared" ref="K184:K188" si="112">IF(C184="", "  "&amp;G184&amp;" = interface", "  "&amp;G184&amp;" = interface(I"&amp;M184&amp;C184&amp;")")</f>
+        <v xml:space="preserve">  ITMDBCache = interface</v>
       </c>
       <c r="L184" s="8" t="str">
-        <f t="shared" si="101"/>
-        <v xml:space="preserve">  TTMDBClient = class(TInterfacedObject, ITMDBClient)</v>
+        <f t="shared" ref="L184:L188" si="113">IF(C184="", "  "&amp;H184&amp;" = class(TInterfacedObject, "&amp;G184&amp;")", "  "&amp;H184&amp;" = class(T"&amp;M184&amp;C184&amp;", "&amp;G184&amp;")")</f>
+        <v xml:space="preserve">  TTMDBCache = class(TInterfacedObject, ITMDBCache)</v>
       </c>
       <c r="M184" s="8" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A185" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="D185" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E185" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="F185" s="14" t="s">
+        <v>377</v>
+      </c>
       <c r="G185" s="8" t="str">
-        <f t="shared" si="98"/>
-        <v>ITMDB</v>
+        <f t="shared" si="110"/>
+        <v>ITMDBLoginState</v>
       </c>
       <c r="H185" s="8" t="str">
-        <f t="shared" si="99"/>
-        <v>TTMDB</v>
+        <f t="shared" si="111"/>
+        <v>TTMDBLoginState</v>
       </c>
       <c r="I185" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDB = interface;</v>
+        <v xml:space="preserve">  ITMDBLoginState = interface;</v>
       </c>
       <c r="J185" s="8" t="str">
         <f t="shared" si="87"/>
-        <v xml:space="preserve">  TTMDB = class;</v>
+        <v xml:space="preserve">  TTMDBLoginState = class;</v>
       </c>
       <c r="K185" s="8" t="str">
-        <f t="shared" si="100"/>
-        <v xml:space="preserve">  ITMDB = interface</v>
+        <f t="shared" si="112"/>
+        <v xml:space="preserve">  ITMDBLoginState = interface</v>
       </c>
       <c r="L185" s="8" t="str">
-        <f t="shared" si="101"/>
-        <v xml:space="preserve">  TTMDB = class(TInterfacedObject, ITMDB)</v>
+        <f t="shared" si="113"/>
+        <v xml:space="preserve">  TTMDBLoginState = class(TInterfacedObject, ITMDBLoginState)</v>
       </c>
       <c r="M185" s="8" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A186" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="D186" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E186" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="F186" s="14" t="s">
+        <v>377</v>
+      </c>
       <c r="G186" s="8" t="str">
-        <f t="shared" si="98"/>
-        <v>ITMDB</v>
+        <f t="shared" si="110"/>
+        <v>ITMDBClient</v>
       </c>
       <c r="H186" s="8" t="str">
-        <f t="shared" si="99"/>
-        <v>TTMDB</v>
+        <f t="shared" si="111"/>
+        <v>TTMDBClient</v>
       </c>
       <c r="I186" s="8" t="str">
         <f t="shared" si="86"/>
-        <v xml:space="preserve">  ITMDB = interface;</v>
+        <v xml:space="preserve">  ITMDBClient = interface;</v>
       </c>
       <c r="J186" s="8" t="str">
         <f t="shared" si="87"/>
+        <v xml:space="preserve">  TTMDBClient = class;</v>
+      </c>
+      <c r="K186" s="8" t="str">
+        <f t="shared" si="112"/>
+        <v xml:space="preserve">  ITMDBClient = interface</v>
+      </c>
+      <c r="L186" s="8" t="str">
+        <f t="shared" si="113"/>
+        <v xml:space="preserve">  TTMDBClient = class(TInterfacedObject, ITMDBClient)</v>
+      </c>
+      <c r="M186" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G187" s="8" t="str">
+        <f t="shared" si="110"/>
+        <v>ITMDB</v>
+      </c>
+      <c r="H187" s="8" t="str">
+        <f t="shared" si="111"/>
+        <v>TTMDB</v>
+      </c>
+      <c r="I187" s="8" t="str">
+        <f t="shared" si="86"/>
+        <v xml:space="preserve">  ITMDB = interface;</v>
+      </c>
+      <c r="J187" s="8" t="str">
+        <f t="shared" si="87"/>
         <v xml:space="preserve">  TTMDB = class;</v>
       </c>
-      <c r="K186" s="8" t="str">
-        <f t="shared" si="100"/>
+      <c r="K187" s="8" t="str">
+        <f t="shared" si="112"/>
         <v xml:space="preserve">  ITMDB = interface</v>
       </c>
-      <c r="L186" s="8" t="str">
-        <f t="shared" si="101"/>
+      <c r="L187" s="8" t="str">
+        <f t="shared" si="113"/>
         <v xml:space="preserve">  TTMDB = class(TInterfacedObject, ITMDB)</v>
       </c>
-      <c r="M186" s="8" t="s">
+      <c r="M187" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G188" s="8" t="str">
+        <f t="shared" si="110"/>
+        <v>ITMDB</v>
+      </c>
+      <c r="H188" s="8" t="str">
+        <f t="shared" si="111"/>
+        <v>TTMDB</v>
+      </c>
+      <c r="I188" s="8" t="str">
+        <f t="shared" si="86"/>
+        <v xml:space="preserve">  ITMDB = interface;</v>
+      </c>
+      <c r="J188" s="8" t="str">
+        <f t="shared" si="87"/>
+        <v xml:space="preserve">  TTMDB = class;</v>
+      </c>
+      <c r="K188" s="8" t="str">
+        <f t="shared" si="112"/>
+        <v xml:space="preserve">  ITMDB = interface</v>
+      </c>
+      <c r="L188" s="8" t="str">
+        <f t="shared" si="113"/>
+        <v xml:space="preserve">  TTMDB = class(TInterfacedObject, ITMDB)</v>
+      </c>
+      <c r="M188" s="8" t="s">
         <v>259</v>
       </c>
     </row>
@@ -14145,25 +14239,25 @@
         <v>269</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>261</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -14171,7 +14265,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C2" t="s">
         <v>280</v>
@@ -14200,7 +14294,7 @@
         <v>140</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C3" t="s">
         <v>276</v>
@@ -14229,7 +14323,7 @@
         <v>140</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -14258,7 +14352,7 @@
         <v>140</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>
@@ -14287,7 +14381,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C6" t="s">
         <v>382</v>
@@ -14316,7 +14410,7 @@
         <v>140</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C7" t="s">
         <v>83</v>
@@ -14345,7 +14439,7 @@
         <v>140</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C8" t="s">
         <v>127</v>
@@ -14374,7 +14468,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -14403,7 +14497,7 @@
         <v>140</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C10" t="s">
         <v>145</v>
@@ -14432,13 +14526,13 @@
         <v>140</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="C11" t="s">
         <v>460</v>
       </c>
-      <c r="C11" t="s">
-        <v>461</v>
-      </c>
       <c r="D11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>377</v>
@@ -14461,7 +14555,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C12" t="s">
         <v>147</v>
@@ -14490,7 +14584,7 @@
         <v>140</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C13" t="s">
         <v>148</v>
@@ -14519,7 +14613,7 @@
         <v>140</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C14" t="s">
         <v>84</v>
@@ -14548,7 +14642,7 @@
         <v>140</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C15" t="s">
         <v>149</v>
@@ -14577,7 +14671,7 @@
         <v>156</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -14606,13 +14700,13 @@
         <v>156</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="C17" t="s">
         <v>462</v>
       </c>
-      <c r="C17" t="s">
-        <v>463</v>
-      </c>
       <c r="D17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>255</v>
@@ -14635,7 +14729,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C18" t="s">
         <v>382</v>
@@ -14664,7 +14758,7 @@
         <v>156</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C19" t="s">
         <v>83</v>
@@ -14693,13 +14787,13 @@
         <v>156</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>255</v>
@@ -14722,13 +14816,13 @@
         <v>156</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C21" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D21" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>255</v>
@@ -14751,7 +14845,7 @@
         <v>156</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
@@ -14780,7 +14874,7 @@
         <v>172</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C23" t="s">
         <v>280</v>
@@ -14809,10 +14903,10 @@
         <v>172</v>
       </c>
       <c r="B24" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="C24" t="s">
         <v>468</v>
-      </c>
-      <c r="C24" t="s">
-        <v>469</v>
       </c>
       <c r="D24" t="s">
         <v>450</v>
@@ -14838,7 +14932,7 @@
         <v>172</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C25" t="s">
         <v>276</v>
@@ -14867,7 +14961,7 @@
         <v>172</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -14896,7 +14990,7 @@
         <v>172</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C27" t="s">
         <v>337</v>
@@ -14925,7 +15019,7 @@
         <v>172</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C28" t="s">
         <v>93</v>
@@ -14954,10 +15048,10 @@
         <v>172</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D29" t="s">
         <v>250</v>
@@ -14983,7 +15077,7 @@
         <v>172</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C30" t="s">
         <v>382</v>
@@ -15012,7 +15106,7 @@
         <v>172</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
@@ -15041,7 +15135,7 @@
         <v>172</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C32" t="s">
         <v>127</v>
@@ -15070,7 +15164,7 @@
         <v>172</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -15099,7 +15193,7 @@
         <v>172</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C34" t="s">
         <v>145</v>
@@ -15128,7 +15222,7 @@
         <v>172</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C35" t="s">
         <v>147</v>
@@ -15157,13 +15251,13 @@
         <v>172</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C36" t="s">
+        <v>470</v>
+      </c>
+      <c r="D36" t="s">
         <v>471</v>
-      </c>
-      <c r="D36" t="s">
-        <v>472</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>255</v>
@@ -15186,7 +15280,7 @@
         <v>172</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C37" t="s">
         <v>148</v>
@@ -15215,7 +15309,7 @@
         <v>172</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C38" t="s">
         <v>84</v>
@@ -15244,7 +15338,7 @@
         <v>172</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C39" t="s">
         <v>149</v>
@@ -15305,7 +15399,7 @@
         <v>451</v>
       </c>
       <c r="C41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D41" t="s">
         <v>450</v>
@@ -15505,7 +15599,7 @@
         <v>178</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C48" t="s">
         <v>280</v>
@@ -15534,7 +15628,7 @@
         <v>178</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -15563,7 +15657,7 @@
         <v>178</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C50" t="s">
         <v>93</v>
@@ -15592,7 +15686,7 @@
         <v>178</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C51" t="s">
         <v>382</v>
@@ -15621,7 +15715,7 @@
         <v>178</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C52" t="s">
         <v>83</v>
@@ -15650,7 +15744,7 @@
         <v>178</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C53" t="s">
         <v>84</v>
@@ -15679,7 +15773,7 @@
         <v>178</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C54" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
Work on Lists #21, code cleanup
Everything in API wrapper implemented except "Lists".
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECDFD2-22A1-4483-987E-33DC1EF174FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51772D3A-DABF-4D25-90E6-C5A1D36D6B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoint Implementation Status" sheetId="1" r:id="rId1"/>
@@ -1994,9 +1994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB394B0-4279-4C9C-A2E8-1B3086916310}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G149" sqref="G149:G150"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,8 +3243,8 @@
       <c r="F54" t="s">
         <v>186</v>
       </c>
-      <c r="G54" s="4" t="s">
-        <v>74</v>
+      <c r="G54" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5551,7 +5551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449EFBB5-22F1-48B7-A5F5-01E59CD1CC21}">
   <dimension ref="A1:M189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
     </sheetView>

</xml_diff>

<commit_message>
HUGE chanches to new tabular test app #45
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51772D3A-DABF-4D25-90E6-C5A1D36D6B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2E29DD-B7D8-4F67-8B7C-8CAA1ED58C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoint Implementation Status" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="494">
   <si>
     <t>Namespace</t>
   </si>
@@ -1416,15 +1416,9 @@
     <t>Interfaced Object</t>
   </si>
   <si>
-    <t>TTMDBMovieDetail</t>
-  </si>
-  <si>
     <t>ReleaseDates</t>
   </si>
   <si>
-    <t>TTMDBPersonDetail</t>
-  </si>
-  <si>
     <t>CombinedCredits</t>
   </si>
   <si>
@@ -1440,9 +1434,6 @@
     <t>ITMDBCombinedCredits</t>
   </si>
   <si>
-    <t>TTMDBTVSerieDetail</t>
-  </si>
-  <si>
     <t>AggregateCredits</t>
   </si>
   <si>
@@ -1455,9 +1446,6 @@
     <t>ITMDBScreenedTheatricallyItems</t>
   </si>
   <si>
-    <t>ITMDBTVEpisodeDetail</t>
-  </si>
-  <si>
     <t>Implementation Signature</t>
   </si>
   <si>
@@ -1519,6 +1507,24 @@
   </si>
   <si>
     <t>ITMDBRatingResult</t>
+  </si>
+  <si>
+    <t>Base Name</t>
+  </si>
+  <si>
+    <t>TMDBMovieDetail</t>
+  </si>
+  <si>
+    <t>TMDBPersonDetail</t>
+  </si>
+  <si>
+    <t>TMDBTVSerieDetail</t>
+  </si>
+  <si>
+    <t>TMDBTVSeasonDetail</t>
+  </si>
+  <si>
+    <t>TMDBTVEpisodeDetail</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1658,6 +1664,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1994,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB394B0-4279-4C9C-A2E8-1B3086916310}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
@@ -3744,7 +3753,7 @@
         <v>207</v>
       </c>
       <c r="F76" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>253</v>
@@ -3767,7 +3776,7 @@
         <v>208</v>
       </c>
       <c r="F77" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>253</v>
@@ -3790,7 +3799,7 @@
         <v>209</v>
       </c>
       <c r="F78" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>253</v>
@@ -3951,7 +3960,7 @@
         <v>220</v>
       </c>
       <c r="F85" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>253</v>
@@ -4043,7 +4052,7 @@
         <v>221</v>
       </c>
       <c r="F89" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>253</v>
@@ -4066,7 +4075,7 @@
         <v>222</v>
       </c>
       <c r="F90" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>253</v>
@@ -4937,7 +4946,7 @@
         <v>207</v>
       </c>
       <c r="F128" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="G128" s="5" t="s">
         <v>253</v>
@@ -4960,7 +4969,7 @@
         <v>208</v>
       </c>
       <c r="F129" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>253</v>
@@ -4983,7 +4992,7 @@
         <v>209</v>
       </c>
       <c r="F130" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G130" s="5" t="s">
         <v>253</v>
@@ -5213,7 +5222,7 @@
         <v>207</v>
       </c>
       <c r="F140" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="G140" s="5" t="s">
         <v>253</v>
@@ -5420,7 +5429,7 @@
         <v>208</v>
       </c>
       <c r="F149" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G149" s="5" t="s">
         <v>253</v>
@@ -5443,7 +5452,7 @@
         <v>209</v>
       </c>
       <c r="F150" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G150" s="5" t="s">
         <v>253</v>
@@ -5552,8 +5561,8 @@
   <dimension ref="A1:M189"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6935,8 +6944,8 @@
       <c r="E31" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>253</v>
+      <c r="F31" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G31" s="8" t="str">
         <f>"I"&amp;M31&amp;B31</f>
@@ -6982,8 +6991,8 @@
       <c r="E32" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>253</v>
+      <c r="F32" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G32" s="8" t="str">
         <f>"I"&amp;M32&amp;B32</f>
@@ -7029,8 +7038,8 @@
       <c r="E33" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>253</v>
+      <c r="F33" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G33" s="8" t="str">
         <f>"I"&amp;M33&amp;B33</f>
@@ -7396,8 +7405,8 @@
       <c r="E41" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F41" s="13" t="s">
-        <v>253</v>
+      <c r="F41" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G41" s="8" t="str">
         <f>"I"&amp;M41&amp;B41</f>
@@ -7537,8 +7546,8 @@
       <c r="E44" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F44" s="13" t="s">
-        <v>253</v>
+      <c r="F44" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G44" s="8" t="str">
         <f>"I"&amp;M44&amp;B44</f>
@@ -7584,8 +7593,8 @@
       <c r="E45" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F45" s="13" t="s">
-        <v>253</v>
+      <c r="F45" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G45" s="8" t="str">
         <f>"I"&amp;M45&amp;B45</f>
@@ -7628,8 +7637,8 @@
       <c r="E46" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F46" s="13" t="s">
-        <v>253</v>
+      <c r="F46" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G46" s="8" t="str">
         <f>"I"&amp;M46&amp;B46</f>
@@ -7675,8 +7684,8 @@
       <c r="E47" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F47" s="13" t="s">
-        <v>253</v>
+      <c r="F47" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G47" s="8" t="str">
         <f>"I"&amp;M47&amp;B47</f>
@@ -7722,8 +7731,8 @@
       <c r="E48" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>253</v>
+      <c r="F48" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G48" s="8" t="str">
         <f>"I"&amp;M48&amp;B48</f>
@@ -8098,8 +8107,8 @@
       <c r="E56" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F56" s="13" t="s">
-        <v>253</v>
+      <c r="F56" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G56" s="8" t="str">
         <f>"I"&amp;M56&amp;B56</f>
@@ -8145,8 +8154,8 @@
       <c r="E57" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F57" s="13" t="s">
-        <v>253</v>
+      <c r="F57" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G57" s="8" t="str">
         <f>"I"&amp;M57&amp;B57</f>
@@ -8192,8 +8201,8 @@
       <c r="E58" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>253</v>
+      <c r="F58" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G58" s="8" t="str">
         <f>"I"&amp;M58&amp;B58</f>
@@ -8239,8 +8248,8 @@
       <c r="E59" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F59" s="13" t="s">
-        <v>253</v>
+      <c r="F59" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G59" s="8" t="str">
         <f>"I"&amp;M59&amp;B59</f>
@@ -8283,8 +8292,8 @@
       <c r="E60" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F60" s="14" t="s">
-        <v>375</v>
+      <c r="F60" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G60" s="8" t="str">
         <f>"I"&amp;M60&amp;B60</f>
@@ -8327,8 +8336,8 @@
       <c r="E61" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F61" s="14" t="s">
-        <v>375</v>
+      <c r="F61" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G61" s="8" t="str">
         <f>"I"&amp;M61&amp;B61</f>
@@ -8371,8 +8380,8 @@
       <c r="E62" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F62" s="14" t="s">
-        <v>375</v>
+      <c r="F62" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G62" s="8" t="str">
         <f>"I"&amp;M62&amp;B62</f>
@@ -8415,8 +8424,8 @@
       <c r="E63" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F63" s="13" t="s">
-        <v>253</v>
+      <c r="F63" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G63" s="8" t="str">
         <f t="shared" si="0"/>
@@ -8462,8 +8471,8 @@
       <c r="E64" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F64" s="13" t="s">
-        <v>253</v>
+      <c r="F64" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G64" s="8" t="str">
         <f t="shared" ref="G64:G77" si="12">"I"&amp;M64&amp;B64</f>
@@ -8509,8 +8518,8 @@
       <c r="E65" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F65" s="13" t="s">
-        <v>253</v>
+      <c r="F65" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G65" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8556,8 +8565,8 @@
       <c r="E66" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F66" s="13" t="s">
-        <v>253</v>
+      <c r="F66" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G66" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8603,8 +8612,8 @@
       <c r="E67" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F67" s="13" t="s">
-        <v>253</v>
+      <c r="F67" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G67" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8650,8 +8659,8 @@
       <c r="E68" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F68" s="13" t="s">
-        <v>253</v>
+      <c r="F68" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G68" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8697,8 +8706,8 @@
       <c r="E69" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F69" s="13" t="s">
-        <v>253</v>
+      <c r="F69" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G69" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8744,8 +8753,8 @@
       <c r="E70" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F70" s="13" t="s">
-        <v>253</v>
+      <c r="F70" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G70" s="8" t="str">
         <f t="shared" si="12"/>
@@ -8791,8 +8800,8 @@
       <c r="E71" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F71" s="13" t="s">
-        <v>253</v>
+      <c r="F71" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="G71" s="8" t="str">
         <f t="shared" si="12"/>
@@ -9106,10 +9115,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D78" s="14" t="s">
         <v>375</v>
@@ -9749,7 +9758,7 @@
         <v>93</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>265</v>
@@ -9796,7 +9805,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>266</v>
@@ -9843,7 +9852,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>265</v>
@@ -9890,7 +9899,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>266</v>
@@ -9937,7 +9946,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>321</v>
@@ -9984,7 +9993,7 @@
         <v>93</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>322</v>
@@ -10031,7 +10040,7 @@
         <v>93</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>323</v>
@@ -10078,7 +10087,7 @@
         <v>93</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>324</v>
@@ -10125,7 +10134,7 @@
         <v>93</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D100" s="14" t="s">
         <v>375</v>
@@ -10169,7 +10178,7 @@
         <v>93</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>270</v>
@@ -10216,7 +10225,7 @@
         <v>93</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>271</v>
@@ -10263,7 +10272,7 @@
         <v>93</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>270</v>
@@ -10310,7 +10319,7 @@
         <v>93</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>271</v>
@@ -10357,7 +10366,7 @@
         <v>93</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>375</v>
@@ -10597,8 +10606,8 @@
       <c r="E110" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F110" s="13" t="s">
-        <v>253</v>
+      <c r="F110" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G110" s="8" t="str">
         <f>"I"&amp;M110&amp;B110</f>
@@ -10644,8 +10653,8 @@
       <c r="E111" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F111" s="13" t="s">
-        <v>253</v>
+      <c r="F111" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G111" s="8" t="str">
         <f>"I"&amp;M111&amp;B111</f>
@@ -10691,8 +10700,8 @@
       <c r="E112" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F112" s="13" t="s">
-        <v>253</v>
+      <c r="F112" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G112" s="8" t="str">
         <f>"I"&amp;M112&amp;B112</f>
@@ -10738,8 +10747,8 @@
       <c r="E113" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F113" s="13" t="s">
-        <v>253</v>
+      <c r="F113" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G113" s="8" t="str">
         <f>"I"&amp;M113&amp;B113</f>
@@ -10829,8 +10838,8 @@
       <c r="E115" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F115" s="14" t="s">
-        <v>375</v>
+      <c r="F115" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G115" s="8" t="str">
         <f t="shared" si="22"/>
@@ -10876,8 +10885,8 @@
       <c r="E116" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F116" s="14" t="s">
-        <v>375</v>
+      <c r="F116" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G116" s="8" t="str">
         <f t="shared" si="22"/>
@@ -10923,8 +10932,8 @@
       <c r="E117" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F117" s="14" t="s">
-        <v>375</v>
+      <c r="F117" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G117" s="8" t="str">
         <f t="shared" si="22"/>
@@ -11611,7 +11620,7 @@
         <v>176</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C132" s="10" t="s">
         <v>265</v>
@@ -11658,7 +11667,7 @@
         <v>176</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C133" s="10" t="s">
         <v>266</v>
@@ -12633,7 +12642,7 @@
         <v>150</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D154" s="14" t="s">
         <v>375</v>
@@ -12677,7 +12686,7 @@
         <v>150</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D155" s="14" t="s">
         <v>375</v>
@@ -12917,8 +12926,8 @@
       <c r="E160" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F160" s="12" t="s">
-        <v>74</v>
+      <c r="F160" s="13" t="s">
+        <v>253</v>
       </c>
       <c r="G160" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13011,8 +13020,8 @@
       <c r="E162" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F162" s="13" t="s">
-        <v>253</v>
+      <c r="F162" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G162" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13105,8 +13114,8 @@
       <c r="E164" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F164" s="12" t="s">
-        <v>74</v>
+      <c r="F164" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G164" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13152,8 +13161,8 @@
       <c r="E165" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F165" s="12" t="s">
-        <v>74</v>
+      <c r="F165" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G165" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13199,8 +13208,8 @@
       <c r="E166" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F166" s="12" t="s">
-        <v>74</v>
+      <c r="F166" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G166" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13381,11 +13390,11 @@
       <c r="C170" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="D170" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E170" s="12" t="s">
-        <v>74</v>
+      <c r="D170" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E170" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="F170" s="12" t="s">
         <v>74</v>
@@ -13434,8 +13443,8 @@
       <c r="E171" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F171" s="12" t="s">
-        <v>74</v>
+      <c r="F171" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G171" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13575,8 +13584,8 @@
       <c r="E174" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F174" s="12" t="s">
-        <v>74</v>
+      <c r="F174" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G174" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13669,8 +13678,8 @@
       <c r="E176" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F176" s="12" t="s">
-        <v>74</v>
+      <c r="F176" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G176" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13716,8 +13725,8 @@
       <c r="E177" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F177" s="14" t="s">
-        <v>375</v>
+      <c r="F177" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G177" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13763,8 +13772,8 @@
       <c r="E178" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F178" s="12" t="s">
-        <v>74</v>
+      <c r="F178" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G178" s="8" t="str">
         <f t="shared" si="94"/>
@@ -13810,8 +13819,8 @@
       <c r="E179" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F179" s="12" t="s">
-        <v>74</v>
+      <c r="F179" s="15" t="s">
+        <v>254</v>
       </c>
       <c r="G179" s="8" t="str">
         <f t="shared" si="94"/>
@@ -14276,9 +14285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31FFFB5-6413-484E-9C48-18C73A8F4597}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14290,7 +14299,7 @@
     <col min="5" max="5" width="9.140625" style="21"/>
     <col min="6" max="6" width="24.140625" style="16" customWidth="1"/>
     <col min="7" max="7" width="79.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="91.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -14301,7 +14310,7 @@
         <v>456</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>259</v>
+        <v>488</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>455</v>
@@ -14313,10 +14322,10 @@
         <v>454</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -14324,7 +14333,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
         <v>278</v>
@@ -14344,8 +14353,8 @@
         <v xml:space="preserve">    function AppendedAccountStates: ITMDBAccountStates; stdcall;</v>
       </c>
       <c r="H2" s="16" t="str">
-        <f>"function T"&amp;B2&amp;"."&amp;F2&amp;": "&amp;D2&amp;";"</f>
-        <v>function TTTMDBMovieDetail.AppendedAccountStates: ITMDBAccountStates;</v>
+        <f>"    function T"&amp;B2&amp;"."&amp;F2&amp;": "&amp;D2&amp;";"</f>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedAccountStates: ITMDBAccountStates;</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -14353,7 +14362,7 @@
         <v>140</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
         <v>274</v>
@@ -14373,8 +14382,8 @@
         <v xml:space="preserve">    function AppendedAlternativeTitles: ITMDBAlternativeTitles; stdcall;</v>
       </c>
       <c r="H3" s="16" t="str">
-        <f t="shared" ref="H3:H54" si="1">"function T"&amp;B3&amp;"."&amp;F3&amp;": "&amp;D3&amp;";"</f>
-        <v>function TTTMDBMovieDetail.AppendedAlternativeTitles: ITMDBAlternativeTitles;</v>
+        <f t="shared" ref="H3:H54" si="1">"    function T"&amp;B3&amp;"."&amp;F3&amp;": "&amp;D3&amp;";"</f>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedAlternativeTitles: ITMDBAlternativeTitles;</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -14382,7 +14391,7 @@
         <v>140</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -14390,7 +14399,7 @@
       <c r="D4" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F4" s="16" t="str">
@@ -14403,7 +14412,7 @@
       </c>
       <c r="H4" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedChanges: ITMDBChanges;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedChanges: ITMDBChanges;</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -14411,7 +14420,7 @@
         <v>140</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>
@@ -14432,7 +14441,7 @@
       </c>
       <c r="H5" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedCredits: ITMDBCredits;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedCredits: ITMDBCredits;</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -14440,7 +14449,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C6" t="s">
         <v>380</v>
@@ -14461,7 +14470,7 @@
       </c>
       <c r="H6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -14469,7 +14478,7 @@
         <v>140</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C7" t="s">
         <v>83</v>
@@ -14490,7 +14499,7 @@
       </c>
       <c r="H7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedImages: ITMDBMediaImageGroup;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedImages: ITMDBMediaImageGroup;</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -14498,7 +14507,7 @@
         <v>140</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C8" t="s">
         <v>127</v>
@@ -14519,7 +14528,7 @@
       </c>
       <c r="H8" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedKeywords: ITMDBKeywords;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedKeywords: ITMDBKeywords;</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -14527,7 +14536,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -14535,7 +14544,7 @@
       <c r="D9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F9" s="16" t="str">
@@ -14548,7 +14557,7 @@
       </c>
       <c r="H9" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedLists: ITMDBListPage;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedLists: ITMDBListPage;</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -14556,7 +14565,7 @@
         <v>140</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C10" t="s">
         <v>145</v>
@@ -14564,7 +14573,7 @@
       <c r="D10" t="s">
         <v>236</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F10" s="16" t="str">
@@ -14577,7 +14586,7 @@
       </c>
       <c r="H10" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedRecommendations: ITMDBMediaPage;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedRecommendations: ITMDBMediaPage;</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -14585,13 +14594,13 @@
         <v>140</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C11" t="s">
         <v>457</v>
       </c>
-      <c r="C11" t="s">
-        <v>458</v>
-      </c>
       <c r="D11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>375</v>
@@ -14606,7 +14615,7 @@
       </c>
       <c r="H11" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedReleaseDates: ITMDBReleaseDates;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedReleaseDates: ITMDBReleaseDates;</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -14614,7 +14623,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C12" t="s">
         <v>147</v>
@@ -14635,7 +14644,7 @@
       </c>
       <c r="H12" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedReviews: ITMDBReviewPage;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedReviews: ITMDBReviewPage;</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -14643,7 +14652,7 @@
         <v>140</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C13" t="s">
         <v>148</v>
@@ -14651,7 +14660,7 @@
       <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F13" s="16" t="str">
@@ -14664,7 +14673,7 @@
       </c>
       <c r="H13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedSimilar: ITMDBMoviePage;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedSimilar: ITMDBMoviePage;</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -14672,7 +14681,7 @@
         <v>140</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C14" t="s">
         <v>84</v>
@@ -14680,7 +14689,7 @@
       <c r="D14" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F14" s="16" t="str">
@@ -14693,7 +14702,7 @@
       </c>
       <c r="H14" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedTranslations: ITMDBTranslations;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedTranslations: ITMDBTranslations;</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -14701,7 +14710,7 @@
         <v>140</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="C15" t="s">
         <v>149</v>
@@ -14722,7 +14731,7 @@
       </c>
       <c r="H15" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBMovieDetail.AppendedVideos: ITMDBVideos;</v>
+        <v xml:space="preserve">    function TTMDBMovieDetail.AppendedVideos: ITMDBVideos;</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -14730,7 +14739,7 @@
         <v>156</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -14738,7 +14747,7 @@
       <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F16" s="16" t="str">
@@ -14751,7 +14760,7 @@
       </c>
       <c r="H16" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedChanges: ITMDBChanges;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedChanges: ITMDBChanges;</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -14759,15 +14768,15 @@
         <v>156</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D17" t="s">
-        <v>464</v>
-      </c>
-      <c r="E17" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F17" s="16" t="str">
@@ -14780,7 +14789,7 @@
       </c>
       <c r="H17" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedCombinedCredits: ITMDBCombinedCredits;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedCombinedCredits: ITMDBCombinedCredits;</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -14788,7 +14797,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C18" t="s">
         <v>380</v>
@@ -14796,7 +14805,7 @@
       <c r="D18" t="s">
         <v>212</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F18" s="16" t="str">
@@ -14809,7 +14818,7 @@
       </c>
       <c r="H18" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -14817,7 +14826,7 @@
         <v>156</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C19" t="s">
         <v>83</v>
@@ -14825,7 +14834,7 @@
       <c r="D19" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F19" s="16" t="str">
@@ -14838,7 +14847,7 @@
       </c>
       <c r="H19" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedImages: ITMDBMediaImageGroup;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedImages: ITMDBMediaImageGroup;</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -14846,15 +14855,15 @@
         <v>156</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="C20" t="s">
         <v>459</v>
       </c>
-      <c r="C20" t="s">
-        <v>461</v>
-      </c>
       <c r="D20" t="s">
-        <v>464</v>
-      </c>
-      <c r="E20" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F20" s="16" t="str">
@@ -14867,7 +14876,7 @@
       </c>
       <c r="H20" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedMovieCredits: ITMDBCombinedCredits;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedMovieCredits: ITMDBCombinedCredits;</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -14875,15 +14884,15 @@
         <v>156</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C21" t="s">
+        <v>460</v>
+      </c>
+      <c r="D21" t="s">
         <v>462</v>
       </c>
-      <c r="D21" t="s">
-        <v>464</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F21" s="16" t="str">
@@ -14896,7 +14905,7 @@
       </c>
       <c r="H21" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedTVCredits: ITMDBCombinedCredits;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedTVCredits: ITMDBCombinedCredits;</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -14904,7 +14913,7 @@
         <v>156</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
@@ -14912,7 +14921,7 @@
       <c r="D22" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F22" s="16" t="str">
@@ -14925,7 +14934,7 @@
       </c>
       <c r="H22" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBPersonDetail.AppendedTranslations: ITMDBTranslations;</v>
+        <v xml:space="preserve">    function TTMDBPersonDetail.AppendedTranslations: ITMDBTranslations;</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -14933,7 +14942,7 @@
         <v>172</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C23" t="s">
         <v>278</v>
@@ -14954,7 +14963,7 @@
       </c>
       <c r="H23" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedAccountStates: ITMDBAccountStates;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedAccountStates: ITMDBAccountStates;</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -14962,15 +14971,15 @@
         <v>172</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C24" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D24" t="s">
         <v>448</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F24" s="16" t="str">
@@ -14983,7 +14992,7 @@
       </c>
       <c r="H24" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedAggregateCredits: ITMDBAggregateCredits;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedAggregateCredits: ITMDBAggregateCredits;</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -14991,7 +15000,7 @@
         <v>172</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C25" t="s">
         <v>274</v>
@@ -15012,7 +15021,7 @@
       </c>
       <c r="H25" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedAlternativeTitles: ITMDBAlternativeTitles;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedAlternativeTitles: ITMDBAlternativeTitles;</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -15020,7 +15029,7 @@
         <v>172</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -15028,7 +15037,7 @@
       <c r="D26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F26" s="16" t="str">
@@ -15041,7 +15050,7 @@
       </c>
       <c r="H26" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedChanges: ITMDBChanges;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedChanges: ITMDBChanges;</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -15049,7 +15058,7 @@
         <v>172</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C27" t="s">
         <v>335</v>
@@ -15057,7 +15066,7 @@
       <c r="D27" t="s">
         <v>247</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F27" s="16" t="str">
@@ -15070,7 +15079,7 @@
       </c>
       <c r="H27" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedContentRatings: ITMDBContentRatings;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedContentRatings: ITMDBContentRatings;</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -15078,7 +15087,7 @@
         <v>172</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C28" t="s">
         <v>93</v>
@@ -15099,7 +15108,7 @@
       </c>
       <c r="H28" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedCredits: ITMDBCredits;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedCredits: ITMDBCredits;</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -15107,15 +15116,15 @@
         <v>172</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C29" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D29" t="s">
         <v>248</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F29" s="16" t="str">
@@ -15128,7 +15137,7 @@
       </c>
       <c r="H29" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedEpisodeGroups: ITMDBEpisodeGroups;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedEpisodeGroups: ITMDBEpisodeGroups;</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -15136,7 +15145,7 @@
         <v>172</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C30" t="s">
         <v>380</v>
@@ -15144,7 +15153,7 @@
       <c r="D30" t="s">
         <v>212</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F30" s="16" t="str">
@@ -15157,7 +15166,7 @@
       </c>
       <c r="H30" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -15165,7 +15174,7 @@
         <v>172</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
@@ -15186,7 +15195,7 @@
       </c>
       <c r="H31" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedImages: ITMDBMediaImageGroup;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedImages: ITMDBMediaImageGroup;</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -15194,7 +15203,7 @@
         <v>172</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C32" t="s">
         <v>127</v>
@@ -15202,7 +15211,7 @@
       <c r="D32" t="s">
         <v>213</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F32" s="16" t="str">
@@ -15215,7 +15224,7 @@
       </c>
       <c r="H32" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedKeywords: ITMDBKeywords;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedKeywords: ITMDBKeywords;</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -15223,7 +15232,7 @@
         <v>172</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -15231,7 +15240,7 @@
       <c r="D33" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F33" s="16" t="str">
@@ -15244,7 +15253,7 @@
       </c>
       <c r="H33" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedLists: ITMDBListPage;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedLists: ITMDBListPage;</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -15252,7 +15261,7 @@
         <v>172</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C34" t="s">
         <v>145</v>
@@ -15260,7 +15269,7 @@
       <c r="D34" t="s">
         <v>236</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F34" s="16" t="str">
@@ -15273,7 +15282,7 @@
       </c>
       <c r="H34" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedRecommendations: ITMDBMediaPage;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedRecommendations: ITMDBMediaPage;</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -15281,7 +15290,7 @@
         <v>172</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C35" t="s">
         <v>147</v>
@@ -15302,7 +15311,7 @@
       </c>
       <c r="H35" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedReviews: ITMDBReviewPage;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedReviews: ITMDBReviewPage;</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -15310,15 +15319,15 @@
         <v>172</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>491</v>
+      </c>
+      <c r="C36" t="s">
         <v>465</v>
       </c>
-      <c r="C36" t="s">
-        <v>468</v>
-      </c>
       <c r="D36" t="s">
-        <v>469</v>
-      </c>
-      <c r="E36" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F36" s="16" t="str">
@@ -15331,7 +15340,7 @@
       </c>
       <c r="H36" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedScreenedTheatrically: ITMDBScreenedTheatricallyItems;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedScreenedTheatrically: ITMDBScreenedTheatricallyItems;</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -15339,7 +15348,7 @@
         <v>172</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C37" t="s">
         <v>148</v>
@@ -15347,7 +15356,7 @@
       <c r="D37" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F37" s="16" t="str">
@@ -15360,7 +15369,7 @@
       </c>
       <c r="H37" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedSimilar: ITMDBTVSeriesPage;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedSimilar: ITMDBTVSeriesPage;</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -15368,7 +15377,7 @@
         <v>172</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C38" t="s">
         <v>84</v>
@@ -15376,7 +15385,7 @@
       <c r="D38" t="s">
         <v>102</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F38" s="16" t="str">
@@ -15389,7 +15398,7 @@
       </c>
       <c r="H38" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedTranslations: ITMDBTranslations;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedTranslations: ITMDBTranslations;</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -15397,7 +15406,7 @@
         <v>172</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="C39" t="s">
         <v>149</v>
@@ -15418,7 +15427,7 @@
       </c>
       <c r="H39" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TTTMDBTVSerieDetail.AppendedVideos: ITMDBVideos;</v>
+        <v xml:space="preserve">    function TTMDBTVSerieDetail.AppendedVideos: ITMDBVideos;</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -15426,7 +15435,7 @@
         <v>177</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C40" t="s">
         <v>278</v>
@@ -15434,7 +15443,7 @@
       <c r="D40" t="s">
         <v>210</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F40" s="16" t="str">
@@ -15447,7 +15456,7 @@
       </c>
       <c r="H40" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedAccountStates: ITMDBAccountStates;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedAccountStates: ITMDBAccountStates;</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -15455,15 +15464,15 @@
         <v>177</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C41" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D41" t="s">
         <v>448</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F41" s="16" t="str">
@@ -15476,7 +15485,7 @@
       </c>
       <c r="H41" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedAggregateCredits: ITMDBAggregateCredits;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedAggregateCredits: ITMDBAggregateCredits;</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -15484,7 +15493,7 @@
         <v>177</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -15492,7 +15501,7 @@
       <c r="D42" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F42" s="16" t="str">
@@ -15505,7 +15514,7 @@
       </c>
       <c r="H42" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedChanges: ITMDBChanges;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedChanges: ITMDBChanges;</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -15513,7 +15522,7 @@
         <v>177</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C43" t="s">
         <v>93</v>
@@ -15521,7 +15530,7 @@
       <c r="D43" t="s">
         <v>211</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F43" s="16" t="str">
@@ -15534,7 +15543,7 @@
       </c>
       <c r="H43" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedCredits: ITMDBCredits;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedCredits: ITMDBCredits;</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -15542,7 +15551,7 @@
         <v>177</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C44" t="s">
         <v>380</v>
@@ -15550,7 +15559,7 @@
       <c r="D44" t="s">
         <v>212</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F44" s="16" t="str">
@@ -15563,7 +15572,7 @@
       </c>
       <c r="H44" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -15571,7 +15580,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -15579,7 +15588,7 @@
       <c r="D45" t="s">
         <v>101</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F45" s="16" t="str">
@@ -15592,7 +15601,7 @@
       </c>
       <c r="H45" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedImages: ITMDBMediaImageGroup;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedImages: ITMDBMediaImageGroup;</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -15600,7 +15609,7 @@
         <v>177</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C46" t="s">
         <v>84</v>
@@ -15608,7 +15617,7 @@
       <c r="D46" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F46" s="16" t="str">
@@ -15621,7 +15630,7 @@
       </c>
       <c r="H46" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedTranslations: ITMDBTranslations;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedTranslations: ITMDBTranslations;</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -15629,7 +15638,7 @@
         <v>177</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="C47" t="s">
         <v>149</v>
@@ -15637,7 +15646,7 @@
       <c r="D47" t="s">
         <v>216</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F47" s="16" t="str">
@@ -15650,7 +15659,7 @@
       </c>
       <c r="H47" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVSeasonDetail.AppendedVideos: ITMDBVideos;</v>
+        <v xml:space="preserve">    function TTMDBTVSeasonDetail.AppendedVideos: ITMDBVideos;</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -15658,7 +15667,7 @@
         <v>178</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C48" t="s">
         <v>278</v>
@@ -15666,7 +15675,7 @@
       <c r="D48" t="s">
         <v>210</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F48" s="16" t="str">
@@ -15679,7 +15688,7 @@
       </c>
       <c r="H48" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedAccountStates: ITMDBAccountStates;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedAccountStates: ITMDBAccountStates;</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -15687,7 +15696,7 @@
         <v>178</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -15695,7 +15704,7 @@
       <c r="D49" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F49" s="16" t="str">
@@ -15708,7 +15717,7 @@
       </c>
       <c r="H49" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedChanges: ITMDBChanges;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedChanges: ITMDBChanges;</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -15716,7 +15725,7 @@
         <v>178</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C50" t="s">
         <v>93</v>
@@ -15724,7 +15733,7 @@
       <c r="D50" t="s">
         <v>211</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F50" s="16" t="str">
@@ -15737,7 +15746,7 @@
       </c>
       <c r="H50" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedCredits: ITMDBCredits;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedCredits: ITMDBCredits;</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -15745,7 +15754,7 @@
         <v>178</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C51" t="s">
         <v>380</v>
@@ -15753,7 +15762,7 @@
       <c r="D51" t="s">
         <v>212</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F51" s="16" t="str">
@@ -15766,7 +15775,7 @@
       </c>
       <c r="H51" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedExternalIDs: ITMDBExternalIDs;</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -15774,7 +15783,7 @@
         <v>178</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C52" t="s">
         <v>83</v>
@@ -15782,7 +15791,7 @@
       <c r="D52" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F52" s="16" t="str">
@@ -15795,7 +15804,7 @@
       </c>
       <c r="H52" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedImages: ITMDBMediaImageGroup;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedImages: ITMDBMediaImageGroup;</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -15803,7 +15812,7 @@
         <v>178</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C53" t="s">
         <v>84</v>
@@ -15811,7 +15820,7 @@
       <c r="D53" t="s">
         <v>102</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F53" s="16" t="str">
@@ -15824,7 +15833,7 @@
       </c>
       <c r="H53" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedTranslations: ITMDBTranslations;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedTranslations: ITMDBTranslations;</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -15832,7 +15841,7 @@
         <v>178</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="C54" t="s">
         <v>149</v>
@@ -15840,7 +15849,7 @@
       <c r="D54" t="s">
         <v>216</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="22" t="s">
         <v>253</v>
       </c>
       <c r="F54" s="16" t="str">
@@ -15853,7 +15862,7 @@
       </c>
       <c r="H54" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>function TITMDBTVEpisodeDetail.AppendedVideos: ITMDBVideos;</v>
+        <v xml:space="preserve">    function TTMDBTVEpisodeDetail.AppendedVideos: ITMDBVideos;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update JD TMDB API Wrapper Progress Tracking.xlsx
</commit_message>
<xml_diff>
--- a/JD TMDB API Wrapper Progress Tracking.xlsx
+++ b/JD TMDB API Wrapper Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\JD-TMDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF18E5B2-1C47-4C09-8429-68796FEC0B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC343AE-7899-417F-AE55-220F6BD37265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{F5B41A47-5D3B-4291-895C-865BB695D835}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoint Implementation Status" sheetId="1" r:id="rId1"/>
@@ -1994,9 +1994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB394B0-4279-4C9C-A2E8-1B3086916310}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,8 +3286,8 @@
       <c r="F56" t="s">
         <v>198</v>
       </c>
-      <c r="G56" s="5" t="s">
-        <v>253</v>
+      <c r="G56" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3309,8 +3309,8 @@
       <c r="F57" t="s">
         <v>53</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>253</v>
+      <c r="G57" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3332,8 +3332,8 @@
       <c r="F58" t="s">
         <v>53</v>
       </c>
-      <c r="G58" s="5" t="s">
-        <v>253</v>
+      <c r="G58" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3355,8 +3355,8 @@
       <c r="F59" t="s">
         <v>198</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>253</v>
+      <c r="G59" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5551,9 +5551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449EFBB5-22F1-48B7-A5F5-01E59CD1CC21}">
   <dimension ref="A1:M189"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F170" sqref="F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10829,8 +10829,8 @@
       <c r="E115" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F115" s="15" t="s">
-        <v>254</v>
+      <c r="F115" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G115" s="8" t="str">
         <f t="shared" si="28"/>
@@ -10876,8 +10876,8 @@
       <c r="E116" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F116" s="15" t="s">
-        <v>254</v>
+      <c r="F116" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G116" s="8" t="str">
         <f t="shared" si="28"/>
@@ -10923,8 +10923,8 @@
       <c r="E117" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F117" s="15" t="s">
-        <v>254</v>
+      <c r="F117" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G117" s="8" t="str">
         <f t="shared" si="28"/>
@@ -11108,8 +11108,8 @@
       <c r="E121" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F121" s="12" t="s">
-        <v>74</v>
+      <c r="F121" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G121" s="8" t="str">
         <f t="shared" si="28"/>
@@ -13434,8 +13434,8 @@
       <c r="E171" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="F171" s="15" t="s">
-        <v>254</v>
+      <c r="F171" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G171" s="8" t="str">
         <f t="shared" si="106"/>

</xml_diff>